<commit_message>
Working on different ways of using MID
</commit_message>
<xml_diff>
--- a/PQ_Challenge_164.xlsx
+++ b/PQ_Challenge_164.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2050D64-386F-47DD-8539-DB38622CC0E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B638029-AC21-45C1-BE57-8F75DBF15474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
   <si>
     <t>Group</t>
   </si>
@@ -202,6 +202,15 @@
   </si>
   <si>
     <t>Column3</t>
+  </si>
+  <si>
+    <t>AB12345</t>
+  </si>
+  <si>
+    <t>CD56789</t>
+  </si>
+  <si>
+    <t>EF01234</t>
   </si>
 </sst>
 </file>
@@ -1020,10 +1029,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U28"/>
+  <dimension ref="A1:W28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+      <selection activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1589,7 +1598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>8</v>
       </c>
@@ -1624,8 +1633,18 @@
       <c r="O17" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="T17" t="s">
+        <v>48</v>
+      </c>
+      <c r="V17" t="str" cm="1">
+        <f t="array" ref="V17:W19">_xlfn.CHOOSECOLS(MID(T17:T19,{1,3,6},{2,3,2}),1,3)</f>
+        <v>AB</v>
+      </c>
+      <c r="W17" t="str">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>13</v>
       </c>
@@ -1660,8 +1679,17 @@
       <c r="O18" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="T18" t="s">
+        <v>49</v>
+      </c>
+      <c r="V18" t="str">
+        <v>CD</v>
+      </c>
+      <c r="W18" t="str">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>22</v>
       </c>
@@ -1696,8 +1724,17 @@
       <c r="O19" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="T19" t="s">
+        <v>50</v>
+      </c>
+      <c r="V19" t="str">
+        <v>EF</v>
+      </c>
+      <c r="W19" t="str">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>43</v>
       </c>
@@ -1733,7 +1770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>44</v>
       </c>
@@ -1769,7 +1806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:23" x14ac:dyDescent="0.3">
       <c r="G22" t="str">
         <v>B</v>
       </c>
@@ -1795,7 +1832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:23" x14ac:dyDescent="0.3">
       <c r="G23" t="str">
         <v>B</v>
       </c>
@@ -1821,7 +1858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:23" x14ac:dyDescent="0.3">
       <c r="G24" t="str">
         <v>B</v>
       </c>
@@ -1847,7 +1884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:23" x14ac:dyDescent="0.3">
       <c r="G25" t="str">
         <v>C</v>
       </c>
@@ -1873,7 +1910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:23" x14ac:dyDescent="0.3">
       <c r="G26" t="str">
         <v>C</v>
       </c>
@@ -1899,7 +1936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:23" x14ac:dyDescent="0.3">
       <c r="G27" t="str">
         <v>C</v>
       </c>
@@ -1925,7 +1962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:23" x14ac:dyDescent="0.3">
       <c r="G28" t="str">
         <v>C</v>
       </c>

</xml_diff>

<commit_message>
Added what I learned
</commit_message>
<xml_diff>
--- a/PQ_Challenge_164.xlsx
+++ b/PQ_Challenge_164.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B638029-AC21-45C1-BE57-8F75DBF15474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516DE33E-1833-4671-BE02-731FFC8FE8CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -749,6 +749,230 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>484094</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>53788</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>224117</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>161365</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{277E8528-8C69-A60D-99F9-84B996E9544F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11322423" y="1129553"/>
+          <a:ext cx="4616823" cy="824753"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>I learned three major things here:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:sym typeface="Webdings" panose="05030102010509060703" pitchFamily="18" charset="2"/>
+            </a:rPr>
+            <a:t> The MID</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:sym typeface="Webdings" panose="05030102010509060703" pitchFamily="18" charset="2"/>
+            </a:rPr>
+            <a:t> trick for extracting multiple groups of different sizes is gold.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+              <a:sym typeface="Webdings" panose="05030102010509060703" pitchFamily="18" charset="2"/>
+            </a:rPr>
+            <a:t></a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> The</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> technique of mapping an array to row lables is excellent.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+              <a:sym typeface="Webdings" panose="05030102010509060703" pitchFamily="18" charset="2"/>
+            </a:rPr>
+            <a:t></a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> Use of TOCOL to unravel columns.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1032,7 +1256,7 @@
   <dimension ref="A1:W28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V18" sqref="V18"/>
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>